<commit_message>
import Utils.X instead of import X
</commit_message>
<xml_diff>
--- a/Output/transcript_domains_DE.xlsx
+++ b/Output/transcript_domains_DE.xlsx
@@ -124,16 +124,16 @@
     <t>VWFA</t>
   </si>
   <si>
-    <t>EGF-like 1</t>
-  </si>
-  <si>
-    <t>EGF-like 2</t>
-  </si>
-  <si>
-    <t>EGF-like 3</t>
-  </si>
-  <si>
-    <t>EGF-like 4</t>
+    <t>I-EGF 1</t>
+  </si>
+  <si>
+    <t>I-EGF 2</t>
+  </si>
+  <si>
+    <t>I-EGF 3</t>
+  </si>
+  <si>
+    <t>I-EGF 4</t>
   </si>
   <si>
     <t>Disordered</t>
@@ -1121,7 +1121,7 @@
         <v>16</v>
       </c>
       <c r="G7">
-        <v>439</v>
+        <v>466</v>
       </c>
       <c r="H7">
         <v>501</v>
@@ -1211,7 +1211,7 @@
         <v>592</v>
       </c>
       <c r="H10">
-        <v>635</v>
+        <v>631</v>
       </c>
       <c r="I10" t="s">
         <v>38</v>
@@ -1711,7 +1711,7 @@
         <v>16</v>
       </c>
       <c r="G7">
-        <v>436</v>
+        <v>463</v>
       </c>
       <c r="H7">
         <v>498</v>
@@ -1801,7 +1801,7 @@
         <v>586</v>
       </c>
       <c r="H10">
-        <v>629</v>
+        <v>625</v>
       </c>
       <c r="I10" t="s">
         <v>38</v>

</xml_diff>